<commit_message>
add tile effect cfg
</commit_message>
<xml_diff>
--- a/Datas/Defines/__tables__.xlsx
+++ b/Datas/Defines/__tables__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SunHeSLGConfigs\Datas\Defines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B251D0-2B18-45E3-8A7E-0381DA4B9C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F01D534-BB59-4A5F-A55C-C7B94723D711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,11 +17,11 @@
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="李翔 - 个人视图" guid="{85AA97A2-0E88-44FC-AA64-9A9DFD668CD7}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="420" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="王树湃 - 个人视图" guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1048" activeSheetId="1"/>
+    <customWorkbookView name="相钰 - 个人视图" guid="{FD691EE8-6D2E-49AD-93D9-3F01820A4257}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="施逸诗 - 个人视图" guid="{C05F3069-328B-4A50-B65B-B559784493CA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="Claymore - Personal View" guid="{4093B011-7051-4A58-8326-8FDDEC4FEF9E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1608" yWindow="-8" windowWidth="1616" windowHeight="868" activeSheetId="1"/>
-    <customWorkbookView name="施逸诗 - 个人视图" guid="{C05F3069-328B-4A50-B65B-B559784493CA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="相钰 - 个人视图" guid="{FD691EE8-6D2E-49AD-93D9-3F01820A4257}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="王树湃 - 个人视图" guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1048" activeSheetId="1"/>
-    <customWorkbookView name="李翔 - 个人视图" guid="{85AA97A2-0E88-44FC-AA64-9A9DFD668CD7}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="420" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>##var</t>
   </si>
@@ -197,6 +197,15 @@
   </si>
   <si>
     <t>Class.xlsx</t>
+  </si>
+  <si>
+    <t>SLG.TileEffect</t>
+  </si>
+  <si>
+    <t>TileEffectData</t>
+  </si>
+  <si>
+    <t>TileEffect.xlsx</t>
   </si>
 </sst>
 </file>
@@ -601,7 +610,7 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -771,7 +780,7 @@
       <c r="E6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G6"/>
@@ -811,8 +820,21 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="2" customFormat="1">
-      <c r="D9"/>
-      <c r="E9"/>
+      <c r="B9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:13" s="2" customFormat="1">
       <c r="D10"/>
@@ -1001,13 +1023,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{4093B011-7051-4A58-8326-8FDDEC4FEF9E}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{85AA97A2-0E88-44FC-AA64-9A9DFD668CD7}" topLeftCell="A16">
+      <selection activeCell="E42" sqref="E42"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{C05F3069-328B-4A50-B65B-B559784493CA}" topLeftCell="A16">
-      <selection activeCell="G39" sqref="G39"/>
+    <customSheetView guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}">
+      <selection activeCell="G10" sqref="G10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -1016,13 +1038,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}">
-      <selection activeCell="G10" sqref="G10"/>
+    <customSheetView guid="{C05F3069-328B-4A50-B65B-B559784493CA}" topLeftCell="A16">
+      <selection activeCell="G39" sqref="G39"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{85AA97A2-0E88-44FC-AA64-9A9DFD668CD7}" topLeftCell="A16">
-      <selection activeCell="E42" sqref="E42"/>
+    <customSheetView guid="{4093B011-7051-4A58-8326-8FDDEC4FEF9E}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
     </customSheetView>

</xml_diff>

<commit_message>
add monopoly Chapter and building configs
</commit_message>
<xml_diff>
--- a/Datas/Defines/__tables__.xlsx
+++ b/Datas/Defines/__tables__.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SunHeSLGConfigs\Datas\Defines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\SunHeSLGConfigs\Datas\Defines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7936827-528F-4188-8A42-E71F5270DB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3B0B4A-B599-4B7C-9757-C54255F03EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="675" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="8100" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Claymore - Personal View" guid="{4093B011-7051-4A58-8326-8FDDEC4FEF9E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1608" yWindow="-8" windowWidth="1616" windowHeight="868" activeSheetId="1"/>
+    <customWorkbookView name="施逸诗 - 个人视图" guid="{C05F3069-328B-4A50-B65B-B559784493CA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="相钰 - 个人视图" guid="{FD691EE8-6D2E-49AD-93D9-3F01820A4257}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="王树湃 - 个人视图" guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1048" activeSheetId="1"/>
     <customWorkbookView name="李翔 - 个人视图" guid="{85AA97A2-0E88-44FC-AA64-9A9DFD668CD7}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="420" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="王树湃 - 个人视图" guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1048" activeSheetId="1"/>
-    <customWorkbookView name="相钰 - 个人视图" guid="{FD691EE8-6D2E-49AD-93D9-3F01820A4257}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="施逸诗 - 个人视图" guid="{C05F3069-328B-4A50-B65B-B559784493CA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Claymore - Personal View" guid="{4093B011-7051-4A58-8326-8FDDEC4FEF9E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1608" yWindow="-8" windowWidth="1616" windowHeight="868" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>##var</t>
   </si>
@@ -215,6 +215,27 @@
   </si>
   <si>
     <t>Skills.xlsx</t>
+  </si>
+  <si>
+    <t>MONO.TbChapter</t>
+  </si>
+  <si>
+    <t>Chapter</t>
+  </si>
+  <si>
+    <t>Chapters@TbChapter.xlsx</t>
+  </si>
+  <si>
+    <t>MONO.TbBuilding</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Buildings@TbChapter.xlsx</t>
+  </si>
+  <si>
+    <t>ID+Level</t>
   </si>
 </sst>
 </file>
@@ -619,7 +640,7 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -628,7 +649,7 @@
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" customWidth="1"/>
+    <col min="5" max="5" width="81.5703125" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="37.140625" customWidth="1"/>
     <col min="8" max="8" width="57.42578125" bestFit="1" customWidth="1"/>
@@ -863,12 +884,38 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="2" customFormat="1">
-      <c r="D11"/>
-      <c r="E11"/>
+      <c r="B11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:13" s="2" customFormat="1">
-      <c r="D12"/>
-      <c r="E12"/>
+      <c r="B12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="13" spans="1:13" s="2" customFormat="1">
       <c r="D13"/>
@@ -1045,13 +1092,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{85AA97A2-0E88-44FC-AA64-9A9DFD668CD7}" topLeftCell="A16">
-      <selection activeCell="E42" sqref="E42"/>
+    <customSheetView guid="{4093B011-7051-4A58-8326-8FDDEC4FEF9E}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}">
-      <selection activeCell="G10" sqref="G10"/>
+    <customSheetView guid="{C05F3069-328B-4A50-B65B-B559784493CA}" topLeftCell="A16">
+      <selection activeCell="G39" sqref="G39"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -1060,13 +1107,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{C05F3069-328B-4A50-B65B-B559784493CA}" topLeftCell="A16">
-      <selection activeCell="G39" sqref="G39"/>
+    <customSheetView guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}">
+      <selection activeCell="G10" sqref="G10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{4093B011-7051-4A58-8326-8FDDEC4FEF9E}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{85AA97A2-0E88-44FC-AA64-9A9DFD668CD7}" topLeftCell="A16">
+      <selection activeCell="E42" sqref="E42"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
     </customSheetView>
@@ -1079,8 +1126,10 @@
     <hyperlink ref="E5" r:id="rId9" display="Language@" xr:uid="{40C75D90-311C-412D-A26C-F16779DEAB91}"/>
     <hyperlink ref="E4" r:id="rId10" xr:uid="{EE9DE100-4B25-4107-94B4-DB9CA82630BF}"/>
     <hyperlink ref="E7" r:id="rId11" xr:uid="{5DDCF3C7-FDDB-4DDA-AC8E-5D9CBCF69C47}"/>
+    <hyperlink ref="E11" r:id="rId12" xr:uid="{983B365B-BAB9-4F6F-9D1D-DDB6C3725F0A}"/>
+    <hyperlink ref="E12" r:id="rId13" xr:uid="{6E6559AC-E9E1-4100-9B7C-3ECFE680C3B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add config table pawns
</commit_message>
<xml_diff>
--- a/Datas/Defines/__tables__.xlsx
+++ b/Datas/Defines/__tables__.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\SunHeSLGConfigs\Datas\Defines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\301410195\Desktop\SunHeSLGConfigs\Datas\Defines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F78835-896B-459B-89D2-783C21033002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E9B2F4-18C3-44F3-8ED4-6E03265C3480}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,30 +17,17 @@
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="李翔 - 个人视图" guid="{85AA97A2-0E88-44FC-AA64-9A9DFD668CD7}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="420" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="王树湃 - 个人视图" guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1048" activeSheetId="1"/>
+    <customWorkbookView name="相钰 - 个人视图" guid="{FD691EE8-6D2E-49AD-93D9-3F01820A4257}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="施逸诗 - 个人视图" guid="{C05F3069-328B-4A50-B65B-B559784493CA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="Claymore - Personal View" guid="{4093B011-7051-4A58-8326-8FDDEC4FEF9E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1608" yWindow="-8" windowWidth="1616" windowHeight="868" activeSheetId="1"/>
-    <customWorkbookView name="施逸诗 - 个人视图" guid="{C05F3069-328B-4A50-B65B-B559784493CA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="相钰 - 个人视图" guid="{FD691EE8-6D2E-49AD-93D9-3F01820A4257}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="王树湃 - 个人视图" guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1048" activeSheetId="1"/>
-    <customWorkbookView name="李翔 - 个人视图" guid="{85AA97A2-0E88-44FC-AA64-9A9DFD668CD7}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="420" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>##var</t>
   </si>
@@ -215,6 +202,15 @@
   </si>
   <si>
     <t>read_schema_from_file</t>
+  </si>
+  <si>
+    <t>SLG.TbPawn</t>
+  </si>
+  <si>
+    <t>PawnData</t>
+  </si>
+  <si>
+    <t>Pawns.xlsx</t>
   </si>
 </sst>
 </file>
@@ -619,7 +615,7 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -863,10 +859,21 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="2" customFormat="1">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:13" s="2" customFormat="1">
       <c r="B12" s="1"/>
@@ -1053,13 +1060,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{4093B011-7051-4A58-8326-8FDDEC4FEF9E}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{85AA97A2-0E88-44FC-AA64-9A9DFD668CD7}" topLeftCell="A16">
+      <selection activeCell="E42" sqref="E42"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{C05F3069-328B-4A50-B65B-B559784493CA}" topLeftCell="A16">
-      <selection activeCell="G39" sqref="G39"/>
+    <customSheetView guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}">
+      <selection activeCell="G10" sqref="G10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -1068,13 +1075,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}">
-      <selection activeCell="G10" sqref="G10"/>
+    <customSheetView guid="{C05F3069-328B-4A50-B65B-B559784493CA}" topLeftCell="A16">
+      <selection activeCell="G39" sqref="G39"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{85AA97A2-0E88-44FC-AA64-9A9DFD668CD7}" topLeftCell="A16">
-      <selection activeCell="E42" sqref="E42"/>
+    <customSheetView guid="{4093B011-7051-4A58-8326-8FDDEC4FEF9E}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
     </customSheetView>

</xml_diff>

<commit_message>
add config for chapter
</commit_message>
<xml_diff>
--- a/Datas/Defines/__tables__.xlsx
+++ b/Datas/Defines/__tables__.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\SunHeSLGConfigs\Datas\Defines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\301410195\Desktop\SunHeSLGConfigs\Datas\Defines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81AA4A2-25CA-4353-8705-1F28C27296F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C63294B-5090-4169-895F-45CC5383E50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7170" yWindow="4305" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Claymore - Personal View" guid="{4093B011-7051-4A58-8326-8FDDEC4FEF9E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1608" yWindow="-8" windowWidth="1616" windowHeight="868" activeSheetId="1"/>
+    <customWorkbookView name="施逸诗 - 个人视图" guid="{C05F3069-328B-4A50-B65B-B559784493CA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="相钰 - 个人视图" guid="{FD691EE8-6D2E-49AD-93D9-3F01820A4257}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="王树湃 - 个人视图" guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1048" activeSheetId="1"/>
     <customWorkbookView name="李翔 - 个人视图" guid="{85AA97A2-0E88-44FC-AA64-9A9DFD668CD7}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="420" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="王树湃 - 个人视图" guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1048" activeSheetId="1"/>
-    <customWorkbookView name="相钰 - 个人视图" guid="{FD691EE8-6D2E-49AD-93D9-3F01820A4257}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="施逸诗 - 个人视图" guid="{C05F3069-328B-4A50-B65B-B559784493CA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Claymore - Personal View" guid="{4093B011-7051-4A58-8326-8FDDEC4FEF9E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1608" yWindow="-8" windowWidth="1616" windowHeight="868" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
   <si>
     <t>##var</t>
   </si>
@@ -274,6 +274,15 @@
   </si>
   <si>
     <t>MapEvent@MonopolyMap.xlsx</t>
+  </si>
+  <si>
+    <t>SLG.TbChapter</t>
+  </si>
+  <si>
+    <t>ChapterData</t>
+  </si>
+  <si>
+    <t>Chapters@TbChapter.xlsx</t>
   </si>
 </sst>
 </file>
@@ -684,24 +693,24 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" customWidth="1"/>
-    <col min="5" max="5" width="46.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="46.7109375" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="37.109375" customWidth="1"/>
-    <col min="8" max="8" width="57.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -1065,6 +1074,24 @@
         <v>41</v>
       </c>
       <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="2"/>
@@ -1209,13 +1236,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{85AA97A2-0E88-44FC-AA64-9A9DFD668CD7}" topLeftCell="A16">
-      <selection activeCell="E42" sqref="E42"/>
+    <customSheetView guid="{4093B011-7051-4A58-8326-8FDDEC4FEF9E}">
+      <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}">
-      <selection activeCell="G10" sqref="G10"/>
+    <customSheetView guid="{C05F3069-328B-4A50-B65B-B559784493CA}" topLeftCell="A16">
+      <selection activeCell="G39" sqref="G39"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -1224,13 +1251,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{C05F3069-328B-4A50-B65B-B559784493CA}" topLeftCell="A16">
-      <selection activeCell="G39" sqref="G39"/>
+    <customSheetView guid="{6DED3B0C-C3F9-407D-BD93-7870E5F8C596}">
+      <selection activeCell="G10" sqref="G10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{4093B011-7051-4A58-8326-8FDDEC4FEF9E}">
-      <selection activeCell="F9" sqref="F9"/>
+    <customSheetView guid="{85AA97A2-0E88-44FC-AA64-9A9DFD668CD7}" topLeftCell="A16">
+      <selection activeCell="E42" sqref="E42"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
     </customSheetView>
@@ -1250,8 +1277,9 @@
     <hyperlink ref="E16" r:id="rId16" xr:uid="{E2F1EBAC-0D5B-4250-AA9E-C6482F26A672}"/>
     <hyperlink ref="E17" r:id="rId17" xr:uid="{F3A12288-5D60-442B-ADC5-CD6189518F13}"/>
     <hyperlink ref="E18" r:id="rId18" xr:uid="{A5047164-56DB-4CFD-B18A-2160443ED195}"/>
+    <hyperlink ref="E19" r:id="rId19" xr:uid="{C50800EA-A37B-4C48-835F-2DBFAA43D58C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>